<commit_message>
added filter for engeeners working on in activity log
</commit_message>
<xml_diff>
--- a/backend-status-burnin/BC Shift Activities.xlsx
+++ b/backend-status-burnin/BC Shift Activities.xlsx
@@ -4,40 +4,40 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Shift 2 - 2025-02-16" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Shift 3 - 2025-02-16" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>2025-02-16</t>
+  </si>
+  <si>
+    <t>EJECUTAR GRR</t>
+  </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Shift</t>
-  </si>
-  <si>
-    <t>Activities</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Engineer</t>
-  </si>
-  <si>
-    <t>2025-02-16</t>
-  </si>
-  <si>
-    <t>EJECUTAR GRR</t>
-  </si>
-  <si>
-    <t>Renato Hacel Cal y Mayor Rodríguez</t>
+    <t>Renato Hacel Cal y Mayor Rodríguez, Usuario de BC</t>
   </si>
 </sst>
 </file>
@@ -54,6 +54,7 @@
     </font>
     <font>
       <b/>
+      <color rgb="FFFFFFFF"/>
     </font>
   </fonts>
   <fills count="3">
@@ -69,7 +70,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,13 +78,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,52 +436,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="39" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="50" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pending add activity log page
</commit_message>
<xml_diff>
--- a/backend-status-burnin/BC Shift Activities.xlsx
+++ b/backend-status-burnin/BC Shift Activities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Shift 3 - 2025-02-16" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Shift 2 - 2025-02-17" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -28,7 +28,7 @@
     <t>Engineer</t>
   </si>
   <si>
-    <t>2025-02-16</t>
+    <t>2025-02-17</t>
   </si>
   <si>
     <t>EJECUTAR GRR</t>
@@ -37,7 +37,7 @@
     <t/>
   </si>
   <si>
-    <t>Renato Hacel Cal y Mayor Rodríguez, Usuario de BC</t>
+    <t>Renato Hacel Cal y Mayor Rodríguez, Usuario de BC, Administrador</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>

</xml_diff>